<commit_message>
1205 cap 3 sum
</commit_message>
<xml_diff>
--- a/projects/psp/refined_data/jvb.xlsx
+++ b/projects/psp/refined_data/jvb.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27430"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3880" yWindow="660" windowWidth="26800" windowHeight="18340" tabRatio="500"/>
+    <workbookView xWindow="6120" yWindow="740" windowWidth="26800" windowHeight="18340" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="jvb_pivot.csv (2)" sheetId="2" r:id="rId1"/>
@@ -586,12 +586,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="cylinder"/>
-        <c:axId val="2131924776"/>
-        <c:axId val="2132748904"/>
+        <c:axId val="-2121131016"/>
+        <c:axId val="-2121142856"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="2131924776"/>
+        <c:axId val="-2121131016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -611,7 +611,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2132748904"/>
+        <c:crossAx val="-2121142856"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -619,7 +619,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2132748904"/>
+        <c:axId val="-2121142856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -630,7 +630,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2131924776"/>
+        <c:crossAx val="-2121131016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1022,7 +1022,7 @@
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12:G18"/>
+      <selection activeCell="B2" sqref="B2:F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>